<commit_message>
ReArrange code into functions and Rename CPUSIM into start script
</commit_message>
<xml_diff>
--- a/memory.xlsx
+++ b/memory.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DACDB6BB-935F-4DD7-9D5A-2D4E2735990B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5134724-4B9D-43C2-AB5F-FA3CF5C067AC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="312" yWindow="312" windowWidth="22728" windowHeight="12048" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="40">
   <si>
     <t>F4</t>
   </si>
@@ -110,28 +110,34 @@
     <t>cycle 5</t>
   </si>
   <si>
-    <t>1C</t>
-  </si>
-  <si>
     <t>cycle 6</t>
   </si>
   <si>
     <t>cycle 7</t>
   </si>
   <si>
-    <t>0C</t>
-  </si>
-  <si>
     <t>cycle 8</t>
-  </si>
-  <si>
-    <t>1E</t>
   </si>
   <si>
     <t>cycle 9</t>
   </si>
   <si>
     <t>cycle 10</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>cycle 11</t>
+  </si>
+  <si>
+    <t>1C</t>
+  </si>
+  <si>
+    <t>0C</t>
+  </si>
+  <si>
+    <t>1E</t>
   </si>
   <si>
     <t>0F</t>
@@ -486,7 +492,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L257"/>
+  <dimension ref="A1:M257"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="L2" sqref="L2:L257"/>
@@ -497,7 +503,7 @@
     <col min="2" max="2" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -520,22 +526,25 @@
         <v>28</v>
       </c>
       <c r="H1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1" t="s">
         <v>30</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>31</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
+        <v>32</v>
+      </c>
+      <c r="L1" t="s">
         <v>33</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>35</v>
       </c>
-      <c r="L1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
@@ -572,8 +581,11 @@
       <c r="L2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -610,13 +622,16 @@
       <c r="L3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
-      <c r="B4" s="1">
-        <v>0</v>
+      <c r="B4" s="1" t="s">
+        <v>34</v>
       </c>
       <c r="C4">
         <v>3</v>
@@ -646,10 +661,13 @@
         <v>3</v>
       </c>
       <c r="L4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+      <c r="M4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
@@ -686,8 +704,11 @@
       <c r="L5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
@@ -724,8 +745,11 @@
       <c r="L6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
@@ -762,8 +786,11 @@
       <c r="L7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
@@ -800,8 +827,11 @@
       <c r="L8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7</v>
       </c>
@@ -838,8 +868,11 @@
       <c r="L9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>8</v>
       </c>
@@ -876,8 +909,11 @@
       <c r="L10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>9</v>
       </c>
@@ -914,8 +950,11 @@
       <c r="L11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10</v>
       </c>
@@ -952,8 +991,11 @@
       <c r="L12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>11</v>
       </c>
@@ -990,8 +1032,11 @@
       <c r="L13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>12</v>
       </c>
@@ -1028,8 +1073,11 @@
       <c r="L14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>13</v>
       </c>
@@ -1066,8 +1114,11 @@
       <c r="L15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>14</v>
       </c>
@@ -1104,8 +1155,11 @@
       <c r="L16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>15</v>
       </c>
@@ -1142,8 +1196,11 @@
       <c r="L17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>16</v>
       </c>
@@ -1180,8 +1237,11 @@
       <c r="L18" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M18" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>17</v>
       </c>
@@ -1218,8 +1278,11 @@
       <c r="L19">
         <v>4</v>
       </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M19">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>18</v>
       </c>
@@ -1256,8 +1319,11 @@
       <c r="L20">
         <v>2</v>
       </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>19</v>
       </c>
@@ -1294,8 +1360,11 @@
       <c r="L21">
         <v>4</v>
       </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M21">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>20</v>
       </c>
@@ -1332,8 +1401,11 @@
       <c r="L22">
         <v>60</v>
       </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M22">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>21</v>
       </c>
@@ -1370,8 +1442,11 @@
       <c r="L23" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M23" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>22</v>
       </c>
@@ -1408,8 +1483,11 @@
       <c r="L24" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M24" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>23</v>
       </c>
@@ -1446,8 +1524,11 @@
       <c r="L25" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M25" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>24</v>
       </c>
@@ -1484,8 +1565,11 @@
       <c r="L26">
         <v>11</v>
       </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M26">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>25</v>
       </c>
@@ -1522,8 +1606,11 @@
       <c r="L27" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M27" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>26</v>
       </c>
@@ -1560,8 +1647,11 @@
       <c r="L28" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M28" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>27</v>
       </c>
@@ -1598,8 +1688,11 @@
       <c r="L29">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>28</v>
       </c>
@@ -1636,8 +1729,11 @@
       <c r="L30" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M30" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>29</v>
       </c>
@@ -1674,8 +1770,11 @@
       <c r="L31" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M31" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>30</v>
       </c>
@@ -1712,8 +1811,11 @@
       <c r="L32" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M32" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>31</v>
       </c>
@@ -1750,8 +1852,11 @@
       <c r="L33" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M33" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>32</v>
       </c>
@@ -1788,8 +1893,11 @@
       <c r="L34">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>33</v>
       </c>
@@ -1826,8 +1934,11 @@
       <c r="L35">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>34</v>
       </c>
@@ -1864,8 +1975,11 @@
       <c r="L36">
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>35</v>
       </c>
@@ -1902,8 +2016,11 @@
       <c r="L37">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>36</v>
       </c>
@@ -1940,8 +2057,11 @@
       <c r="L38">
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>37</v>
       </c>
@@ -1978,8 +2098,11 @@
       <c r="L39">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>38</v>
       </c>
@@ -2016,8 +2139,11 @@
       <c r="L40">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>39</v>
       </c>
@@ -2054,8 +2180,11 @@
       <c r="L41">
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>40</v>
       </c>
@@ -2092,8 +2221,11 @@
       <c r="L42">
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>41</v>
       </c>
@@ -2130,8 +2262,11 @@
       <c r="L43">
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>42</v>
       </c>
@@ -2168,8 +2303,11 @@
       <c r="L44">
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>43</v>
       </c>
@@ -2206,8 +2344,11 @@
       <c r="L45">
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>44</v>
       </c>
@@ -2244,8 +2385,11 @@
       <c r="L46">
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>45</v>
       </c>
@@ -2282,8 +2426,11 @@
       <c r="L47">
         <v>0</v>
       </c>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>46</v>
       </c>
@@ -2320,8 +2467,11 @@
       <c r="L48">
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>47</v>
       </c>
@@ -2358,8 +2508,11 @@
       <c r="L49">
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>48</v>
       </c>
@@ -2396,8 +2549,11 @@
       <c r="L50">
         <v>0</v>
       </c>
-    </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>49</v>
       </c>
@@ -2434,8 +2590,11 @@
       <c r="L51">
         <v>0</v>
       </c>
-    </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>50</v>
       </c>
@@ -2472,8 +2631,11 @@
       <c r="L52">
         <v>0</v>
       </c>
-    </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>51</v>
       </c>
@@ -2510,8 +2672,11 @@
       <c r="L53">
         <v>0</v>
       </c>
-    </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>52</v>
       </c>
@@ -2548,8 +2713,11 @@
       <c r="L54">
         <v>0</v>
       </c>
-    </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>53</v>
       </c>
@@ -2586,8 +2754,11 @@
       <c r="L55">
         <v>0</v>
       </c>
-    </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>54</v>
       </c>
@@ -2624,8 +2795,11 @@
       <c r="L56">
         <v>0</v>
       </c>
-    </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>55</v>
       </c>
@@ -2662,8 +2836,11 @@
       <c r="L57">
         <v>0</v>
       </c>
-    </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>56</v>
       </c>
@@ -2700,8 +2877,11 @@
       <c r="L58">
         <v>0</v>
       </c>
-    </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>57</v>
       </c>
@@ -2738,8 +2918,11 @@
       <c r="L59">
         <v>0</v>
       </c>
-    </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>58</v>
       </c>
@@ -2776,8 +2959,11 @@
       <c r="L60">
         <v>0</v>
       </c>
-    </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>59</v>
       </c>
@@ -2814,8 +3000,11 @@
       <c r="L61">
         <v>0</v>
       </c>
-    </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>60</v>
       </c>
@@ -2852,8 +3041,11 @@
       <c r="L62">
         <v>0</v>
       </c>
-    </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>61</v>
       </c>
@@ -2890,8 +3082,11 @@
       <c r="L63">
         <v>0</v>
       </c>
-    </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>62</v>
       </c>
@@ -2928,8 +3123,11 @@
       <c r="L64">
         <v>0</v>
       </c>
-    </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>63</v>
       </c>
@@ -2966,8 +3164,11 @@
       <c r="L65">
         <v>0</v>
       </c>
-    </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>64</v>
       </c>
@@ -3004,8 +3205,11 @@
       <c r="L66">
         <v>0</v>
       </c>
-    </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>65</v>
       </c>
@@ -3042,8 +3246,11 @@
       <c r="L67">
         <v>0</v>
       </c>
-    </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>66</v>
       </c>
@@ -3080,8 +3287,11 @@
       <c r="L68">
         <v>0</v>
       </c>
-    </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>67</v>
       </c>
@@ -3118,8 +3328,11 @@
       <c r="L69">
         <v>0</v>
       </c>
-    </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>68</v>
       </c>
@@ -3156,8 +3369,11 @@
       <c r="L70">
         <v>0</v>
       </c>
-    </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>69</v>
       </c>
@@ -3194,8 +3410,11 @@
       <c r="L71">
         <v>0</v>
       </c>
-    </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>70</v>
       </c>
@@ -3232,8 +3451,11 @@
       <c r="L72">
         <v>0</v>
       </c>
-    </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>71</v>
       </c>
@@ -3270,8 +3492,11 @@
       <c r="L73">
         <v>0</v>
       </c>
-    </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>72</v>
       </c>
@@ -3308,8 +3533,11 @@
       <c r="L74">
         <v>0</v>
       </c>
-    </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>73</v>
       </c>
@@ -3346,8 +3574,11 @@
       <c r="L75">
         <v>0</v>
       </c>
-    </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>74</v>
       </c>
@@ -3384,8 +3615,11 @@
       <c r="L76">
         <v>0</v>
       </c>
-    </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>75</v>
       </c>
@@ -3422,8 +3656,11 @@
       <c r="L77">
         <v>0</v>
       </c>
-    </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>76</v>
       </c>
@@ -3460,8 +3697,11 @@
       <c r="L78">
         <v>0</v>
       </c>
-    </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>77</v>
       </c>
@@ -3498,8 +3738,11 @@
       <c r="L79">
         <v>0</v>
       </c>
-    </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M79">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>78</v>
       </c>
@@ -3536,8 +3779,11 @@
       <c r="L80">
         <v>0</v>
       </c>
-    </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>79</v>
       </c>
@@ -3574,8 +3820,11 @@
       <c r="L81">
         <v>0</v>
       </c>
-    </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M81">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>80</v>
       </c>
@@ -3612,8 +3861,11 @@
       <c r="L82">
         <v>0</v>
       </c>
-    </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M82">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>81</v>
       </c>
@@ -3650,8 +3902,11 @@
       <c r="L83">
         <v>0</v>
       </c>
-    </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M83">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>82</v>
       </c>
@@ -3688,8 +3943,11 @@
       <c r="L84">
         <v>0</v>
       </c>
-    </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>83</v>
       </c>
@@ -3726,8 +3984,11 @@
       <c r="L85">
         <v>0</v>
       </c>
-    </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M85">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>84</v>
       </c>
@@ -3764,8 +4025,11 @@
       <c r="L86">
         <v>0</v>
       </c>
-    </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M86">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>85</v>
       </c>
@@ -3802,8 +4066,11 @@
       <c r="L87">
         <v>0</v>
       </c>
-    </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>86</v>
       </c>
@@ -3840,8 +4107,11 @@
       <c r="L88">
         <v>0</v>
       </c>
-    </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M88">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>87</v>
       </c>
@@ -3878,8 +4148,11 @@
       <c r="L89">
         <v>0</v>
       </c>
-    </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M89">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>88</v>
       </c>
@@ -3916,8 +4189,11 @@
       <c r="L90">
         <v>0</v>
       </c>
-    </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M90">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>89</v>
       </c>
@@ -3954,8 +4230,11 @@
       <c r="L91">
         <v>0</v>
       </c>
-    </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M91">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>90</v>
       </c>
@@ -3992,8 +4271,11 @@
       <c r="L92">
         <v>0</v>
       </c>
-    </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M92">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>91</v>
       </c>
@@ -4030,8 +4312,11 @@
       <c r="L93">
         <v>0</v>
       </c>
-    </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M93">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>92</v>
       </c>
@@ -4068,8 +4353,11 @@
       <c r="L94">
         <v>0</v>
       </c>
-    </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M94">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>93</v>
       </c>
@@ -4106,8 +4394,11 @@
       <c r="L95">
         <v>0</v>
       </c>
-    </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M95">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>94</v>
       </c>
@@ -4144,8 +4435,11 @@
       <c r="L96">
         <v>0</v>
       </c>
-    </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M96">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>95</v>
       </c>
@@ -4182,8 +4476,11 @@
       <c r="L97">
         <v>0</v>
       </c>
-    </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M97">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>96</v>
       </c>
@@ -4220,8 +4517,11 @@
       <c r="L98">
         <v>0</v>
       </c>
-    </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M98">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>97</v>
       </c>
@@ -4258,8 +4558,11 @@
       <c r="L99">
         <v>0</v>
       </c>
-    </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M99">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>98</v>
       </c>
@@ -4296,8 +4599,11 @@
       <c r="L100">
         <v>0</v>
       </c>
-    </row>
-    <row r="101" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M100">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>99</v>
       </c>
@@ -4334,8 +4640,11 @@
       <c r="L101">
         <v>0</v>
       </c>
-    </row>
-    <row r="102" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M101">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>100</v>
       </c>
@@ -4372,8 +4681,11 @@
       <c r="L102">
         <v>0</v>
       </c>
-    </row>
-    <row r="103" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M102">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A103">
         <v>101</v>
       </c>
@@ -4410,8 +4722,11 @@
       <c r="L103">
         <v>0</v>
       </c>
-    </row>
-    <row r="104" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M103">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A104">
         <v>102</v>
       </c>
@@ -4448,8 +4763,11 @@
       <c r="L104">
         <v>0</v>
       </c>
-    </row>
-    <row r="105" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M104">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A105">
         <v>103</v>
       </c>
@@ -4486,8 +4804,11 @@
       <c r="L105">
         <v>0</v>
       </c>
-    </row>
-    <row r="106" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M105">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>104</v>
       </c>
@@ -4524,8 +4845,11 @@
       <c r="L106">
         <v>0</v>
       </c>
-    </row>
-    <row r="107" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M106">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A107">
         <v>105</v>
       </c>
@@ -4562,8 +4886,11 @@
       <c r="L107">
         <v>0</v>
       </c>
-    </row>
-    <row r="108" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M107">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A108">
         <v>106</v>
       </c>
@@ -4600,8 +4927,11 @@
       <c r="L108">
         <v>0</v>
       </c>
-    </row>
-    <row r="109" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M108">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A109">
         <v>107</v>
       </c>
@@ -4638,8 +4968,11 @@
       <c r="L109">
         <v>0</v>
       </c>
-    </row>
-    <row r="110" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M109">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A110">
         <v>108</v>
       </c>
@@ -4676,8 +5009,11 @@
       <c r="L110">
         <v>0</v>
       </c>
-    </row>
-    <row r="111" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A111">
         <v>109</v>
       </c>
@@ -4714,8 +5050,11 @@
       <c r="L111">
         <v>0</v>
       </c>
-    </row>
-    <row r="112" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M111">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A112">
         <v>110</v>
       </c>
@@ -4752,8 +5091,11 @@
       <c r="L112">
         <v>0</v>
       </c>
-    </row>
-    <row r="113" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M112">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A113">
         <v>111</v>
       </c>
@@ -4790,8 +5132,11 @@
       <c r="L113">
         <v>0</v>
       </c>
-    </row>
-    <row r="114" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M113">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A114">
         <v>112</v>
       </c>
@@ -4828,8 +5173,11 @@
       <c r="L114">
         <v>0</v>
       </c>
-    </row>
-    <row r="115" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M114">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A115">
         <v>113</v>
       </c>
@@ -4866,8 +5214,11 @@
       <c r="L115">
         <v>0</v>
       </c>
-    </row>
-    <row r="116" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M115">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A116">
         <v>114</v>
       </c>
@@ -4904,8 +5255,11 @@
       <c r="L116">
         <v>0</v>
       </c>
-    </row>
-    <row r="117" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M116">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A117">
         <v>115</v>
       </c>
@@ -4942,8 +5296,11 @@
       <c r="L117">
         <v>0</v>
       </c>
-    </row>
-    <row r="118" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M117">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A118">
         <v>116</v>
       </c>
@@ -4980,8 +5337,11 @@
       <c r="L118">
         <v>0</v>
       </c>
-    </row>
-    <row r="119" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M118">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A119">
         <v>117</v>
       </c>
@@ -5018,8 +5378,11 @@
       <c r="L119">
         <v>0</v>
       </c>
-    </row>
-    <row r="120" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M119">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A120">
         <v>118</v>
       </c>
@@ -5056,8 +5419,11 @@
       <c r="L120">
         <v>0</v>
       </c>
-    </row>
-    <row r="121" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M120">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A121">
         <v>119</v>
       </c>
@@ -5094,8 +5460,11 @@
       <c r="L121">
         <v>0</v>
       </c>
-    </row>
-    <row r="122" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M121">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A122">
         <v>120</v>
       </c>
@@ -5132,8 +5501,11 @@
       <c r="L122">
         <v>0</v>
       </c>
-    </row>
-    <row r="123" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M122">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A123">
         <v>121</v>
       </c>
@@ -5170,8 +5542,11 @@
       <c r="L123">
         <v>0</v>
       </c>
-    </row>
-    <row r="124" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M123">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A124">
         <v>122</v>
       </c>
@@ -5208,8 +5583,11 @@
       <c r="L124">
         <v>0</v>
       </c>
-    </row>
-    <row r="125" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M124">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A125">
         <v>123</v>
       </c>
@@ -5246,8 +5624,11 @@
       <c r="L125">
         <v>0</v>
       </c>
-    </row>
-    <row r="126" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M125">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A126">
         <v>124</v>
       </c>
@@ -5284,8 +5665,11 @@
       <c r="L126">
         <v>0</v>
       </c>
-    </row>
-    <row r="127" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M126">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A127">
         <v>125</v>
       </c>
@@ -5322,8 +5706,11 @@
       <c r="L127">
         <v>0</v>
       </c>
-    </row>
-    <row r="128" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M127">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A128">
         <v>126</v>
       </c>
@@ -5360,8 +5747,11 @@
       <c r="L128">
         <v>0</v>
       </c>
-    </row>
-    <row r="129" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M128">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A129">
         <v>127</v>
       </c>
@@ -5398,8 +5788,11 @@
       <c r="L129">
         <v>0</v>
       </c>
-    </row>
-    <row r="130" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M129">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A130">
         <v>128</v>
       </c>
@@ -5436,8 +5829,11 @@
       <c r="L130">
         <v>0</v>
       </c>
-    </row>
-    <row r="131" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M130">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A131">
         <v>129</v>
       </c>
@@ -5474,8 +5870,11 @@
       <c r="L131">
         <v>0</v>
       </c>
-    </row>
-    <row r="132" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M131">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A132">
         <v>130</v>
       </c>
@@ -5512,8 +5911,11 @@
       <c r="L132">
         <v>0</v>
       </c>
-    </row>
-    <row r="133" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M132">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A133">
         <v>131</v>
       </c>
@@ -5550,8 +5952,11 @@
       <c r="L133">
         <v>0</v>
       </c>
-    </row>
-    <row r="134" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M133">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A134">
         <v>132</v>
       </c>
@@ -5588,8 +5993,11 @@
       <c r="L134">
         <v>0</v>
       </c>
-    </row>
-    <row r="135" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M134">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A135">
         <v>133</v>
       </c>
@@ -5626,8 +6034,11 @@
       <c r="L135">
         <v>0</v>
       </c>
-    </row>
-    <row r="136" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M135">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A136">
         <v>134</v>
       </c>
@@ -5664,8 +6075,11 @@
       <c r="L136">
         <v>0</v>
       </c>
-    </row>
-    <row r="137" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M136">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A137">
         <v>135</v>
       </c>
@@ -5702,8 +6116,11 @@
       <c r="L137">
         <v>0</v>
       </c>
-    </row>
-    <row r="138" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M137">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A138">
         <v>136</v>
       </c>
@@ -5740,8 +6157,11 @@
       <c r="L138">
         <v>0</v>
       </c>
-    </row>
-    <row r="139" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M138">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A139">
         <v>137</v>
       </c>
@@ -5778,8 +6198,11 @@
       <c r="L139">
         <v>0</v>
       </c>
-    </row>
-    <row r="140" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M139">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A140">
         <v>138</v>
       </c>
@@ -5816,8 +6239,11 @@
       <c r="L140">
         <v>0</v>
       </c>
-    </row>
-    <row r="141" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M140">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="141" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A141">
         <v>139</v>
       </c>
@@ -5854,8 +6280,11 @@
       <c r="L141">
         <v>0</v>
       </c>
-    </row>
-    <row r="142" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M141">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="142" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A142">
         <v>140</v>
       </c>
@@ -5892,8 +6321,11 @@
       <c r="L142">
         <v>0</v>
       </c>
-    </row>
-    <row r="143" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M142">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="143" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A143">
         <v>141</v>
       </c>
@@ -5930,8 +6362,11 @@
       <c r="L143">
         <v>0</v>
       </c>
-    </row>
-    <row r="144" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M143">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="144" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A144">
         <v>142</v>
       </c>
@@ -5968,8 +6403,11 @@
       <c r="L144">
         <v>0</v>
       </c>
-    </row>
-    <row r="145" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M144">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="145" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A145">
         <v>143</v>
       </c>
@@ -6006,8 +6444,11 @@
       <c r="L145">
         <v>0</v>
       </c>
-    </row>
-    <row r="146" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M145">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="146" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A146">
         <v>144</v>
       </c>
@@ -6044,8 +6485,11 @@
       <c r="L146">
         <v>0</v>
       </c>
-    </row>
-    <row r="147" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M146">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="147" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A147">
         <v>145</v>
       </c>
@@ -6082,8 +6526,11 @@
       <c r="L147">
         <v>0</v>
       </c>
-    </row>
-    <row r="148" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M147">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="148" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A148">
         <v>146</v>
       </c>
@@ -6120,8 +6567,11 @@
       <c r="L148">
         <v>0</v>
       </c>
-    </row>
-    <row r="149" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M148">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="149" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A149">
         <v>147</v>
       </c>
@@ -6158,8 +6608,11 @@
       <c r="L149">
         <v>0</v>
       </c>
-    </row>
-    <row r="150" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M149">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="150" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A150">
         <v>148</v>
       </c>
@@ -6196,8 +6649,11 @@
       <c r="L150">
         <v>0</v>
       </c>
-    </row>
-    <row r="151" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M150">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="151" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A151">
         <v>149</v>
       </c>
@@ -6234,8 +6690,11 @@
       <c r="L151">
         <v>0</v>
       </c>
-    </row>
-    <row r="152" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M151">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="152" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A152">
         <v>150</v>
       </c>
@@ -6272,8 +6731,11 @@
       <c r="L152">
         <v>0</v>
       </c>
-    </row>
-    <row r="153" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M152">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="153" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A153">
         <v>151</v>
       </c>
@@ -6310,8 +6772,11 @@
       <c r="L153">
         <v>0</v>
       </c>
-    </row>
-    <row r="154" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M153">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="154" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A154">
         <v>152</v>
       </c>
@@ -6348,8 +6813,11 @@
       <c r="L154">
         <v>0</v>
       </c>
-    </row>
-    <row r="155" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M154">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="155" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A155">
         <v>153</v>
       </c>
@@ -6386,8 +6854,11 @@
       <c r="L155">
         <v>0</v>
       </c>
-    </row>
-    <row r="156" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M155">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="156" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A156">
         <v>154</v>
       </c>
@@ -6424,8 +6895,11 @@
       <c r="L156">
         <v>0</v>
       </c>
-    </row>
-    <row r="157" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M156">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="157" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A157">
         <v>155</v>
       </c>
@@ -6462,8 +6936,11 @@
       <c r="L157">
         <v>0</v>
       </c>
-    </row>
-    <row r="158" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M157">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="158" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A158">
         <v>156</v>
       </c>
@@ -6500,8 +6977,11 @@
       <c r="L158">
         <v>0</v>
       </c>
-    </row>
-    <row r="159" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M158">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="159" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A159">
         <v>157</v>
       </c>
@@ -6538,8 +7018,11 @@
       <c r="L159">
         <v>0</v>
       </c>
-    </row>
-    <row r="160" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M159">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="160" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A160">
         <v>158</v>
       </c>
@@ -6576,8 +7059,11 @@
       <c r="L160">
         <v>0</v>
       </c>
-    </row>
-    <row r="161" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M160">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="161" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A161">
         <v>159</v>
       </c>
@@ -6614,8 +7100,11 @@
       <c r="L161">
         <v>0</v>
       </c>
-    </row>
-    <row r="162" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M161">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="162" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A162">
         <v>160</v>
       </c>
@@ -6652,8 +7141,11 @@
       <c r="L162">
         <v>0</v>
       </c>
-    </row>
-    <row r="163" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M162">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="163" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A163">
         <v>161</v>
       </c>
@@ -6690,8 +7182,11 @@
       <c r="L163">
         <v>0</v>
       </c>
-    </row>
-    <row r="164" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M163">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="164" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A164">
         <v>162</v>
       </c>
@@ -6728,8 +7223,11 @@
       <c r="L164">
         <v>0</v>
       </c>
-    </row>
-    <row r="165" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M164">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="165" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A165">
         <v>163</v>
       </c>
@@ -6766,8 +7264,11 @@
       <c r="L165">
         <v>0</v>
       </c>
-    </row>
-    <row r="166" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M165">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="166" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A166">
         <v>164</v>
       </c>
@@ -6804,8 +7305,11 @@
       <c r="L166">
         <v>0</v>
       </c>
-    </row>
-    <row r="167" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M166">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="167" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A167">
         <v>165</v>
       </c>
@@ -6842,8 +7346,11 @@
       <c r="L167">
         <v>0</v>
       </c>
-    </row>
-    <row r="168" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M167">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="168" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A168">
         <v>166</v>
       </c>
@@ -6880,8 +7387,11 @@
       <c r="L168">
         <v>0</v>
       </c>
-    </row>
-    <row r="169" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M168">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="169" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A169">
         <v>167</v>
       </c>
@@ -6918,8 +7428,11 @@
       <c r="L169">
         <v>0</v>
       </c>
-    </row>
-    <row r="170" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M169">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="170" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A170">
         <v>168</v>
       </c>
@@ -6956,8 +7469,11 @@
       <c r="L170">
         <v>0</v>
       </c>
-    </row>
-    <row r="171" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M170">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="171" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A171">
         <v>169</v>
       </c>
@@ -6994,8 +7510,11 @@
       <c r="L171">
         <v>0</v>
       </c>
-    </row>
-    <row r="172" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M171">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="172" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A172">
         <v>170</v>
       </c>
@@ -7032,8 +7551,11 @@
       <c r="L172">
         <v>0</v>
       </c>
-    </row>
-    <row r="173" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M172">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="173" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A173">
         <v>171</v>
       </c>
@@ -7070,8 +7592,11 @@
       <c r="L173">
         <v>0</v>
       </c>
-    </row>
-    <row r="174" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M173">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="174" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A174">
         <v>172</v>
       </c>
@@ -7108,8 +7633,11 @@
       <c r="L174">
         <v>0</v>
       </c>
-    </row>
-    <row r="175" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M174">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="175" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A175">
         <v>173</v>
       </c>
@@ -7146,8 +7674,11 @@
       <c r="L175">
         <v>0</v>
       </c>
-    </row>
-    <row r="176" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M175">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="176" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A176">
         <v>174</v>
       </c>
@@ -7184,8 +7715,11 @@
       <c r="L176">
         <v>0</v>
       </c>
-    </row>
-    <row r="177" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M176">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="177" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A177">
         <v>175</v>
       </c>
@@ -7222,8 +7756,11 @@
       <c r="L177">
         <v>0</v>
       </c>
-    </row>
-    <row r="178" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M177">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="178" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A178">
         <v>176</v>
       </c>
@@ -7260,8 +7797,11 @@
       <c r="L178">
         <v>0</v>
       </c>
-    </row>
-    <row r="179" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M178">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="179" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A179">
         <v>177</v>
       </c>
@@ -7298,8 +7838,11 @@
       <c r="L179">
         <v>0</v>
       </c>
-    </row>
-    <row r="180" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M179">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="180" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A180">
         <v>178</v>
       </c>
@@ -7336,8 +7879,11 @@
       <c r="L180">
         <v>0</v>
       </c>
-    </row>
-    <row r="181" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M180">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="181" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A181">
         <v>179</v>
       </c>
@@ -7374,8 +7920,11 @@
       <c r="L181">
         <v>0</v>
       </c>
-    </row>
-    <row r="182" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M181">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="182" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A182">
         <v>180</v>
       </c>
@@ -7412,8 +7961,11 @@
       <c r="L182">
         <v>0</v>
       </c>
-    </row>
-    <row r="183" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M182">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="183" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A183">
         <v>181</v>
       </c>
@@ -7450,8 +8002,11 @@
       <c r="L183">
         <v>0</v>
       </c>
-    </row>
-    <row r="184" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M183">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="184" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A184">
         <v>182</v>
       </c>
@@ -7488,8 +8043,11 @@
       <c r="L184">
         <v>0</v>
       </c>
-    </row>
-    <row r="185" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M184">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="185" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A185">
         <v>183</v>
       </c>
@@ -7526,8 +8084,11 @@
       <c r="L185">
         <v>0</v>
       </c>
-    </row>
-    <row r="186" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M185">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="186" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A186">
         <v>184</v>
       </c>
@@ -7564,8 +8125,11 @@
       <c r="L186">
         <v>0</v>
       </c>
-    </row>
-    <row r="187" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M186">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="187" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A187">
         <v>185</v>
       </c>
@@ -7602,8 +8166,11 @@
       <c r="L187">
         <v>0</v>
       </c>
-    </row>
-    <row r="188" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M187">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="188" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A188">
         <v>186</v>
       </c>
@@ -7640,8 +8207,11 @@
       <c r="L188">
         <v>0</v>
       </c>
-    </row>
-    <row r="189" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M188">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="189" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A189">
         <v>187</v>
       </c>
@@ -7678,8 +8248,11 @@
       <c r="L189">
         <v>0</v>
       </c>
-    </row>
-    <row r="190" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M189">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="190" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A190">
         <v>188</v>
       </c>
@@ -7716,8 +8289,11 @@
       <c r="L190">
         <v>0</v>
       </c>
-    </row>
-    <row r="191" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M190">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="191" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A191">
         <v>189</v>
       </c>
@@ -7754,8 +8330,11 @@
       <c r="L191">
         <v>0</v>
       </c>
-    </row>
-    <row r="192" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M191">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="192" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A192">
         <v>190</v>
       </c>
@@ -7792,8 +8371,11 @@
       <c r="L192">
         <v>0</v>
       </c>
-    </row>
-    <row r="193" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M192">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="193" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A193">
         <v>191</v>
       </c>
@@ -7830,8 +8412,11 @@
       <c r="L193">
         <v>0</v>
       </c>
-    </row>
-    <row r="194" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M193">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="194" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A194">
         <v>192</v>
       </c>
@@ -7868,8 +8453,11 @@
       <c r="L194">
         <v>0</v>
       </c>
-    </row>
-    <row r="195" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M194">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="195" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A195">
         <v>193</v>
       </c>
@@ -7906,8 +8494,11 @@
       <c r="L195">
         <v>0</v>
       </c>
-    </row>
-    <row r="196" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M195">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="196" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A196">
         <v>194</v>
       </c>
@@ -7944,8 +8535,11 @@
       <c r="L196">
         <v>0</v>
       </c>
-    </row>
-    <row r="197" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M196">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="197" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A197">
         <v>195</v>
       </c>
@@ -7982,8 +8576,11 @@
       <c r="L197">
         <v>0</v>
       </c>
-    </row>
-    <row r="198" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M197">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="198" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A198">
         <v>196</v>
       </c>
@@ -8020,8 +8617,11 @@
       <c r="L198">
         <v>0</v>
       </c>
-    </row>
-    <row r="199" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M198">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="199" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A199">
         <v>197</v>
       </c>
@@ -8058,8 +8658,11 @@
       <c r="L199">
         <v>0</v>
       </c>
-    </row>
-    <row r="200" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M199">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="200" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A200">
         <v>198</v>
       </c>
@@ -8096,8 +8699,11 @@
       <c r="L200">
         <v>0</v>
       </c>
-    </row>
-    <row r="201" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M200">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="201" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A201">
         <v>199</v>
       </c>
@@ -8134,8 +8740,11 @@
       <c r="L201">
         <v>0</v>
       </c>
-    </row>
-    <row r="202" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M201">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="202" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A202">
         <v>200</v>
       </c>
@@ -8172,8 +8781,11 @@
       <c r="L202">
         <v>0</v>
       </c>
-    </row>
-    <row r="203" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M202">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="203" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A203">
         <v>201</v>
       </c>
@@ -8210,8 +8822,11 @@
       <c r="L203">
         <v>0</v>
       </c>
-    </row>
-    <row r="204" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M203">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="204" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A204">
         <v>202</v>
       </c>
@@ -8248,8 +8863,11 @@
       <c r="L204">
         <v>0</v>
       </c>
-    </row>
-    <row r="205" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M204">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="205" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A205">
         <v>203</v>
       </c>
@@ -8286,8 +8904,11 @@
       <c r="L205">
         <v>0</v>
       </c>
-    </row>
-    <row r="206" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M205">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="206" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A206">
         <v>204</v>
       </c>
@@ -8324,8 +8945,11 @@
       <c r="L206">
         <v>0</v>
       </c>
-    </row>
-    <row r="207" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M206">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="207" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A207">
         <v>205</v>
       </c>
@@ -8362,8 +8986,11 @@
       <c r="L207">
         <v>0</v>
       </c>
-    </row>
-    <row r="208" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M207">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="208" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A208">
         <v>206</v>
       </c>
@@ -8400,8 +9027,11 @@
       <c r="L208">
         <v>0</v>
       </c>
-    </row>
-    <row r="209" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M208">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="209" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A209">
         <v>207</v>
       </c>
@@ -8438,8 +9068,11 @@
       <c r="L209">
         <v>0</v>
       </c>
-    </row>
-    <row r="210" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M209">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="210" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A210">
         <v>208</v>
       </c>
@@ -8476,8 +9109,11 @@
       <c r="L210">
         <v>0</v>
       </c>
-    </row>
-    <row r="211" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M210">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="211" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A211">
         <v>209</v>
       </c>
@@ -8514,8 +9150,11 @@
       <c r="L211">
         <v>0</v>
       </c>
-    </row>
-    <row r="212" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M211">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="212" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A212">
         <v>210</v>
       </c>
@@ -8552,8 +9191,11 @@
       <c r="L212">
         <v>0</v>
       </c>
-    </row>
-    <row r="213" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M212">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="213" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A213">
         <v>211</v>
       </c>
@@ -8590,8 +9232,11 @@
       <c r="L213">
         <v>0</v>
       </c>
-    </row>
-    <row r="214" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M213">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="214" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A214">
         <v>212</v>
       </c>
@@ -8628,8 +9273,11 @@
       <c r="L214">
         <v>0</v>
       </c>
-    </row>
-    <row r="215" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M214">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="215" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A215">
         <v>213</v>
       </c>
@@ -8666,8 +9314,11 @@
       <c r="L215">
         <v>0</v>
       </c>
-    </row>
-    <row r="216" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M215">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="216" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A216">
         <v>214</v>
       </c>
@@ -8704,8 +9355,11 @@
       <c r="L216">
         <v>0</v>
       </c>
-    </row>
-    <row r="217" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M216">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="217" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A217">
         <v>215</v>
       </c>
@@ -8742,8 +9396,11 @@
       <c r="L217">
         <v>0</v>
       </c>
-    </row>
-    <row r="218" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M217">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="218" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A218">
         <v>216</v>
       </c>
@@ -8780,8 +9437,11 @@
       <c r="L218">
         <v>0</v>
       </c>
-    </row>
-    <row r="219" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M218">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="219" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A219">
         <v>217</v>
       </c>
@@ -8818,8 +9478,11 @@
       <c r="L219">
         <v>0</v>
       </c>
-    </row>
-    <row r="220" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M219">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="220" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A220">
         <v>218</v>
       </c>
@@ -8856,8 +9519,11 @@
       <c r="L220">
         <v>0</v>
       </c>
-    </row>
-    <row r="221" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M220">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="221" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A221">
         <v>219</v>
       </c>
@@ -8894,8 +9560,11 @@
       <c r="L221">
         <v>0</v>
       </c>
-    </row>
-    <row r="222" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M221">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="222" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A222">
         <v>220</v>
       </c>
@@ -8932,8 +9601,11 @@
       <c r="L222">
         <v>0</v>
       </c>
-    </row>
-    <row r="223" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M222">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="223" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A223">
         <v>221</v>
       </c>
@@ -8970,8 +9642,11 @@
       <c r="L223">
         <v>0</v>
       </c>
-    </row>
-    <row r="224" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M223">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="224" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A224">
         <v>222</v>
       </c>
@@ -9008,8 +9683,11 @@
       <c r="L224">
         <v>0</v>
       </c>
-    </row>
-    <row r="225" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M224">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="225" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A225">
         <v>223</v>
       </c>
@@ -9046,8 +9724,11 @@
       <c r="L225">
         <v>0</v>
       </c>
-    </row>
-    <row r="226" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M225">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="226" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A226">
         <v>224</v>
       </c>
@@ -9084,8 +9765,11 @@
       <c r="L226">
         <v>0</v>
       </c>
-    </row>
-    <row r="227" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M226">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="227" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A227">
         <v>225</v>
       </c>
@@ -9122,8 +9806,11 @@
       <c r="L227">
         <v>0</v>
       </c>
-    </row>
-    <row r="228" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M227">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="228" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A228">
         <v>226</v>
       </c>
@@ -9160,8 +9847,11 @@
       <c r="L228">
         <v>0</v>
       </c>
-    </row>
-    <row r="229" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M228">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="229" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A229">
         <v>227</v>
       </c>
@@ -9198,8 +9888,11 @@
       <c r="L229">
         <v>0</v>
       </c>
-    </row>
-    <row r="230" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M229">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="230" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A230">
         <v>228</v>
       </c>
@@ -9236,8 +9929,11 @@
       <c r="L230">
         <v>0</v>
       </c>
-    </row>
-    <row r="231" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M230">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="231" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A231">
         <v>229</v>
       </c>
@@ -9274,8 +9970,11 @@
       <c r="L231">
         <v>0</v>
       </c>
-    </row>
-    <row r="232" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M231">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="232" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A232">
         <v>230</v>
       </c>
@@ -9312,8 +10011,11 @@
       <c r="L232">
         <v>0</v>
       </c>
-    </row>
-    <row r="233" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M232">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="233" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A233">
         <v>231</v>
       </c>
@@ -9350,8 +10052,11 @@
       <c r="L233">
         <v>0</v>
       </c>
-    </row>
-    <row r="234" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M233">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="234" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A234">
         <v>232</v>
       </c>
@@ -9388,8 +10093,11 @@
       <c r="L234">
         <v>0</v>
       </c>
-    </row>
-    <row r="235" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M234">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="235" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A235">
         <v>233</v>
       </c>
@@ -9426,8 +10134,11 @@
       <c r="L235">
         <v>0</v>
       </c>
-    </row>
-    <row r="236" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M235">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="236" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A236">
         <v>234</v>
       </c>
@@ -9464,8 +10175,11 @@
       <c r="L236">
         <v>0</v>
       </c>
-    </row>
-    <row r="237" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M236">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="237" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A237">
         <v>235</v>
       </c>
@@ -9502,8 +10216,11 @@
       <c r="L237">
         <v>0</v>
       </c>
-    </row>
-    <row r="238" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M237">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="238" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A238">
         <v>236</v>
       </c>
@@ -9540,8 +10257,11 @@
       <c r="L238">
         <v>0</v>
       </c>
-    </row>
-    <row r="239" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M238">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="239" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A239">
         <v>237</v>
       </c>
@@ -9578,8 +10298,11 @@
       <c r="L239">
         <v>0</v>
       </c>
-    </row>
-    <row r="240" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M239">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="240" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A240">
         <v>238</v>
       </c>
@@ -9616,8 +10339,11 @@
       <c r="L240">
         <v>0</v>
       </c>
-    </row>
-    <row r="241" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M240">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="241" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A241">
         <v>239</v>
       </c>
@@ -9654,8 +10380,11 @@
       <c r="L241">
         <v>0</v>
       </c>
-    </row>
-    <row r="242" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M241">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="242" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A242">
         <v>240</v>
       </c>
@@ -9692,8 +10421,11 @@
       <c r="L242">
         <v>0</v>
       </c>
-    </row>
-    <row r="243" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M242">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="243" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A243">
         <v>241</v>
       </c>
@@ -9730,8 +10462,11 @@
       <c r="L243">
         <v>0</v>
       </c>
-    </row>
-    <row r="244" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M243">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="244" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A244">
         <v>242</v>
       </c>
@@ -9768,8 +10503,11 @@
       <c r="L244">
         <v>0</v>
       </c>
-    </row>
-    <row r="245" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M244">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="245" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A245">
         <v>243</v>
       </c>
@@ -9806,8 +10544,11 @@
       <c r="L245">
         <v>0</v>
       </c>
-    </row>
-    <row r="246" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M245">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="246" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A246">
         <v>244</v>
       </c>
@@ -9844,8 +10585,11 @@
       <c r="L246">
         <v>0</v>
       </c>
-    </row>
-    <row r="247" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M246">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="247" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A247">
         <v>245</v>
       </c>
@@ -9882,8 +10626,11 @@
       <c r="L247">
         <v>0</v>
       </c>
-    </row>
-    <row r="248" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M247">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="248" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A248">
         <v>246</v>
       </c>
@@ -9920,8 +10667,11 @@
       <c r="L248">
         <v>0</v>
       </c>
-    </row>
-    <row r="249" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M248">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="249" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A249">
         <v>247</v>
       </c>
@@ -9958,8 +10708,11 @@
       <c r="L249">
         <v>0</v>
       </c>
-    </row>
-    <row r="250" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M249">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="250" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A250">
         <v>248</v>
       </c>
@@ -9996,8 +10749,11 @@
       <c r="L250">
         <v>0</v>
       </c>
-    </row>
-    <row r="251" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M250">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="251" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A251">
         <v>249</v>
       </c>
@@ -10034,8 +10790,11 @@
       <c r="L251">
         <v>0</v>
       </c>
-    </row>
-    <row r="252" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M251">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="252" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A252">
         <v>250</v>
       </c>
@@ -10072,8 +10831,11 @@
       <c r="L252">
         <v>0</v>
       </c>
-    </row>
-    <row r="253" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M252">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="253" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A253">
         <v>251</v>
       </c>
@@ -10110,8 +10872,11 @@
       <c r="L253">
         <v>0</v>
       </c>
-    </row>
-    <row r="254" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M253">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="254" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A254">
         <v>252</v>
       </c>
@@ -10148,8 +10913,11 @@
       <c r="L254">
         <v>0</v>
       </c>
-    </row>
-    <row r="255" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M254">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="255" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A255">
         <v>253</v>
       </c>
@@ -10186,13 +10954,16 @@
       <c r="L255">
         <v>0</v>
       </c>
-    </row>
-    <row r="256" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M255">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="256" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A256">
         <v>254</v>
       </c>
-      <c r="B256" s="1">
-        <v>0</v>
+      <c r="B256" t="s">
+        <v>24</v>
       </c>
       <c r="C256" t="s">
         <v>24</v>
@@ -10224,8 +10995,11 @@
       <c r="L256">
         <v>17</v>
       </c>
-    </row>
-    <row r="257" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M256">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="257" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A257">
         <v>255</v>
       </c>
@@ -10260,6 +11034,9 @@
         <v>0</v>
       </c>
       <c r="L257">
+        <v>0</v>
+      </c>
+      <c r="M257">
         <v>0</v>
       </c>
     </row>
@@ -10270,7 +11047,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33C90694-17B9-4987-A12B-4F203B0E59C7}">
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="L2" sqref="L2:L5"/>
@@ -10278,7 +11055,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>15</v>
       </c>
@@ -10298,22 +11075,25 @@
         <v>28</v>
       </c>
       <c r="H1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1" t="s">
         <v>30</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>31</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
+        <v>32</v>
+      </c>
+      <c r="L1" t="s">
         <v>33</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>35</v>
       </c>
-      <c r="L1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -10333,16 +11113,16 @@
         <v>5</v>
       </c>
       <c r="G2" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="H2" t="s">
         <v>5</v>
       </c>
       <c r="I2" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="J2" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="K2">
         <v>17</v>
@@ -10351,7 +11131,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -10389,7 +11169,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -10427,7 +11207,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -10453,16 +11233,16 @@
         <v>6</v>
       </c>
       <c r="I5" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="J5" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="K5" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="L5" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Indent and comment TwoOperand function
</commit_message>
<xml_diff>
--- a/memory.xlsx
+++ b/memory.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5134724-4B9D-43C2-AB5F-FA3CF5C067AC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC8B2B03-9B44-4639-AB32-B6693DC2B99E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="312" yWindow="312" windowWidth="22728" windowHeight="12048" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="40">
   <si>
     <t>F4</t>
   </si>
@@ -495,7 +495,7 @@
   <dimension ref="A1:M257"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L2" sqref="L2:L257"/>
+      <selection activeCell="M2" sqref="M2:M257"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -663,8 +663,8 @@
       <c r="L4" t="s">
         <v>39</v>
       </c>
-      <c r="M4">
-        <v>3</v>
+      <c r="M4" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
@@ -11050,7 +11050,7 @@
   <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2:L5"/>
+      <selection activeCell="M2" sqref="M2:M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11130,6 +11130,9 @@
       <c r="L2">
         <v>19</v>
       </c>
+      <c r="M2" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -11168,6 +11171,9 @@
       <c r="L3" t="s">
         <v>8</v>
       </c>
+      <c r="M3" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -11206,6 +11212,9 @@
       <c r="L4">
         <v>0</v>
       </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -11242,6 +11251,9 @@
         <v>37</v>
       </c>
       <c r="L5" t="s">
+        <v>37</v>
+      </c>
+      <c r="M5" t="s">
         <v>37</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Separate write to Excel function
</commit_message>
<xml_diff>
--- a/memory.xlsx
+++ b/memory.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3B5630E-4553-42F7-88BF-130DD8A4AC3A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB04E790-0285-4AB3-A7DD-8389BA255F16}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="312" yWindow="312" windowWidth="22728" windowHeight="12048" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="41">
   <si>
     <t>F4</t>
   </si>
@@ -137,10 +137,13 @@
     <t>0C</t>
   </si>
   <si>
+    <t>0F</t>
+  </si>
+  <si>
     <t>1E</t>
   </si>
   <si>
-    <t>0F</t>
+    <t>cycle 12</t>
   </si>
 </sst>
 </file>
@@ -492,7 +495,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M257"/>
+  <dimension ref="A1:N257"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="M2" sqref="M2:M257"/>
@@ -503,7 +506,7 @@
     <col min="2" max="2" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -543,8 +546,11 @@
       <c r="M1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
@@ -584,8 +590,11 @@
       <c r="M2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -625,8 +634,11 @@
       <c r="M3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -661,13 +673,16 @@
         <v>3</v>
       </c>
       <c r="L4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+      <c r="N4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
@@ -707,8 +722,11 @@
       <c r="M5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
@@ -748,8 +766,11 @@
       <c r="M6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
@@ -789,8 +810,11 @@
       <c r="M7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
@@ -830,8 +854,11 @@
       <c r="M8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7</v>
       </c>
@@ -871,8 +898,11 @@
       <c r="M9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>8</v>
       </c>
@@ -912,8 +942,11 @@
       <c r="M10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>9</v>
       </c>
@@ -953,8 +986,11 @@
       <c r="M11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10</v>
       </c>
@@ -994,8 +1030,11 @@
       <c r="M12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>11</v>
       </c>
@@ -1035,8 +1074,11 @@
       <c r="M13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>12</v>
       </c>
@@ -1076,8 +1118,11 @@
       <c r="M14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>13</v>
       </c>
@@ -1117,8 +1162,11 @@
       <c r="M15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>14</v>
       </c>
@@ -1158,8 +1206,11 @@
       <c r="M16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>15</v>
       </c>
@@ -1199,8 +1250,11 @@
       <c r="M17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>16</v>
       </c>
@@ -1240,8 +1294,11 @@
       <c r="M18" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N18" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>17</v>
       </c>
@@ -1281,8 +1338,11 @@
       <c r="M19">
         <v>4</v>
       </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N19">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>18</v>
       </c>
@@ -1322,8 +1382,11 @@
       <c r="M20">
         <v>2</v>
       </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>19</v>
       </c>
@@ -1363,8 +1426,11 @@
       <c r="M21">
         <v>4</v>
       </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N21">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>20</v>
       </c>
@@ -1404,8 +1470,11 @@
       <c r="M22">
         <v>60</v>
       </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N22">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>21</v>
       </c>
@@ -1445,8 +1514,11 @@
       <c r="M23" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N23" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>22</v>
       </c>
@@ -1486,8 +1558,11 @@
       <c r="M24" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N24" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>23</v>
       </c>
@@ -1527,8 +1602,11 @@
       <c r="M25" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N25" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>24</v>
       </c>
@@ -1568,8 +1646,11 @@
       <c r="M26">
         <v>11</v>
       </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N26">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>25</v>
       </c>
@@ -1609,8 +1690,11 @@
       <c r="M27" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N27" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>26</v>
       </c>
@@ -1650,8 +1734,11 @@
       <c r="M28" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N28" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>27</v>
       </c>
@@ -1691,8 +1778,11 @@
       <c r="M29">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>28</v>
       </c>
@@ -1732,8 +1822,11 @@
       <c r="M30" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N30" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>29</v>
       </c>
@@ -1773,8 +1866,11 @@
       <c r="M31" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N31" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>30</v>
       </c>
@@ -1814,8 +1910,11 @@
       <c r="M32" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N32" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>31</v>
       </c>
@@ -1855,8 +1954,11 @@
       <c r="M33" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N33" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>32</v>
       </c>
@@ -1896,8 +1998,11 @@
       <c r="M34">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>33</v>
       </c>
@@ -1937,8 +2042,11 @@
       <c r="M35">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>34</v>
       </c>
@@ -1978,8 +2086,11 @@
       <c r="M36">
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>35</v>
       </c>
@@ -2019,8 +2130,11 @@
       <c r="M37">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>36</v>
       </c>
@@ -2060,8 +2174,11 @@
       <c r="M38">
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>37</v>
       </c>
@@ -2101,8 +2218,11 @@
       <c r="M39">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>38</v>
       </c>
@@ -2142,8 +2262,11 @@
       <c r="M40">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>39</v>
       </c>
@@ -2183,8 +2306,11 @@
       <c r="M41">
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>40</v>
       </c>
@@ -2224,8 +2350,11 @@
       <c r="M42">
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>41</v>
       </c>
@@ -2265,8 +2394,11 @@
       <c r="M43">
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>42</v>
       </c>
@@ -2306,8 +2438,11 @@
       <c r="M44">
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>43</v>
       </c>
@@ -2347,8 +2482,11 @@
       <c r="M45">
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>44</v>
       </c>
@@ -2388,8 +2526,11 @@
       <c r="M46">
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>45</v>
       </c>
@@ -2429,8 +2570,11 @@
       <c r="M47">
         <v>0</v>
       </c>
-    </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>46</v>
       </c>
@@ -2470,8 +2614,11 @@
       <c r="M48">
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>47</v>
       </c>
@@ -2511,8 +2658,11 @@
       <c r="M49">
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>48</v>
       </c>
@@ -2552,8 +2702,11 @@
       <c r="M50">
         <v>0</v>
       </c>
-    </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>49</v>
       </c>
@@ -2593,8 +2746,11 @@
       <c r="M51">
         <v>0</v>
       </c>
-    </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>50</v>
       </c>
@@ -2634,8 +2790,11 @@
       <c r="M52">
         <v>0</v>
       </c>
-    </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>51</v>
       </c>
@@ -2675,8 +2834,11 @@
       <c r="M53">
         <v>0</v>
       </c>
-    </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>52</v>
       </c>
@@ -2716,8 +2878,11 @@
       <c r="M54">
         <v>0</v>
       </c>
-    </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>53</v>
       </c>
@@ -2757,8 +2922,11 @@
       <c r="M55">
         <v>0</v>
       </c>
-    </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>54</v>
       </c>
@@ -2798,8 +2966,11 @@
       <c r="M56">
         <v>0</v>
       </c>
-    </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>55</v>
       </c>
@@ -2839,8 +3010,11 @@
       <c r="M57">
         <v>0</v>
       </c>
-    </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>56</v>
       </c>
@@ -2880,8 +3054,11 @@
       <c r="M58">
         <v>0</v>
       </c>
-    </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>57</v>
       </c>
@@ -2921,8 +3098,11 @@
       <c r="M59">
         <v>0</v>
       </c>
-    </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>58</v>
       </c>
@@ -2962,8 +3142,11 @@
       <c r="M60">
         <v>0</v>
       </c>
-    </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>59</v>
       </c>
@@ -3003,8 +3186,11 @@
       <c r="M61">
         <v>0</v>
       </c>
-    </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>60</v>
       </c>
@@ -3044,8 +3230,11 @@
       <c r="M62">
         <v>0</v>
       </c>
-    </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>61</v>
       </c>
@@ -3085,8 +3274,11 @@
       <c r="M63">
         <v>0</v>
       </c>
-    </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>62</v>
       </c>
@@ -3126,8 +3318,11 @@
       <c r="M64">
         <v>0</v>
       </c>
-    </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>63</v>
       </c>
@@ -3167,8 +3362,11 @@
       <c r="M65">
         <v>0</v>
       </c>
-    </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>64</v>
       </c>
@@ -3208,8 +3406,11 @@
       <c r="M66">
         <v>0</v>
       </c>
-    </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>65</v>
       </c>
@@ -3249,8 +3450,11 @@
       <c r="M67">
         <v>0</v>
       </c>
-    </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>66</v>
       </c>
@@ -3290,8 +3494,11 @@
       <c r="M68">
         <v>0</v>
       </c>
-    </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>67</v>
       </c>
@@ -3331,8 +3538,11 @@
       <c r="M69">
         <v>0</v>
       </c>
-    </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>68</v>
       </c>
@@ -3372,8 +3582,11 @@
       <c r="M70">
         <v>0</v>
       </c>
-    </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>69</v>
       </c>
@@ -3413,8 +3626,11 @@
       <c r="M71">
         <v>0</v>
       </c>
-    </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>70</v>
       </c>
@@ -3454,8 +3670,11 @@
       <c r="M72">
         <v>0</v>
       </c>
-    </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>71</v>
       </c>
@@ -3495,8 +3714,11 @@
       <c r="M73">
         <v>0</v>
       </c>
-    </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>72</v>
       </c>
@@ -3536,8 +3758,11 @@
       <c r="M74">
         <v>0</v>
       </c>
-    </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>73</v>
       </c>
@@ -3577,8 +3802,11 @@
       <c r="M75">
         <v>0</v>
       </c>
-    </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>74</v>
       </c>
@@ -3618,8 +3846,11 @@
       <c r="M76">
         <v>0</v>
       </c>
-    </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>75</v>
       </c>
@@ -3659,8 +3890,11 @@
       <c r="M77">
         <v>0</v>
       </c>
-    </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>76</v>
       </c>
@@ -3700,8 +3934,11 @@
       <c r="M78">
         <v>0</v>
       </c>
-    </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>77</v>
       </c>
@@ -3741,8 +3978,11 @@
       <c r="M79">
         <v>0</v>
       </c>
-    </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N79">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>78</v>
       </c>
@@ -3782,8 +4022,11 @@
       <c r="M80">
         <v>0</v>
       </c>
-    </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>79</v>
       </c>
@@ -3823,8 +4066,11 @@
       <c r="M81">
         <v>0</v>
       </c>
-    </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N81">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>80</v>
       </c>
@@ -3864,8 +4110,11 @@
       <c r="M82">
         <v>0</v>
       </c>
-    </row>
-    <row r="83" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N82">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>81</v>
       </c>
@@ -3905,8 +4154,11 @@
       <c r="M83">
         <v>0</v>
       </c>
-    </row>
-    <row r="84" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N83">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>82</v>
       </c>
@@ -3946,8 +4198,11 @@
       <c r="M84">
         <v>0</v>
       </c>
-    </row>
-    <row r="85" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>83</v>
       </c>
@@ -3987,8 +4242,11 @@
       <c r="M85">
         <v>0</v>
       </c>
-    </row>
-    <row r="86" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N85">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>84</v>
       </c>
@@ -4028,8 +4286,11 @@
       <c r="M86">
         <v>0</v>
       </c>
-    </row>
-    <row r="87" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N86">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>85</v>
       </c>
@@ -4069,8 +4330,11 @@
       <c r="M87">
         <v>0</v>
       </c>
-    </row>
-    <row r="88" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>86</v>
       </c>
@@ -4110,8 +4374,11 @@
       <c r="M88">
         <v>0</v>
       </c>
-    </row>
-    <row r="89" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N88">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>87</v>
       </c>
@@ -4151,8 +4418,11 @@
       <c r="M89">
         <v>0</v>
       </c>
-    </row>
-    <row r="90" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N89">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>88</v>
       </c>
@@ -4192,8 +4462,11 @@
       <c r="M90">
         <v>0</v>
       </c>
-    </row>
-    <row r="91" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N90">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>89</v>
       </c>
@@ -4233,8 +4506,11 @@
       <c r="M91">
         <v>0</v>
       </c>
-    </row>
-    <row r="92" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N91">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>90</v>
       </c>
@@ -4274,8 +4550,11 @@
       <c r="M92">
         <v>0</v>
       </c>
-    </row>
-    <row r="93" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N92">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>91</v>
       </c>
@@ -4315,8 +4594,11 @@
       <c r="M93">
         <v>0</v>
       </c>
-    </row>
-    <row r="94" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N93">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>92</v>
       </c>
@@ -4356,8 +4638,11 @@
       <c r="M94">
         <v>0</v>
       </c>
-    </row>
-    <row r="95" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N94">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>93</v>
       </c>
@@ -4397,8 +4682,11 @@
       <c r="M95">
         <v>0</v>
       </c>
-    </row>
-    <row r="96" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N95">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>94</v>
       </c>
@@ -4438,8 +4726,11 @@
       <c r="M96">
         <v>0</v>
       </c>
-    </row>
-    <row r="97" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N96">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>95</v>
       </c>
@@ -4479,8 +4770,11 @@
       <c r="M97">
         <v>0</v>
       </c>
-    </row>
-    <row r="98" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N97">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>96</v>
       </c>
@@ -4520,8 +4814,11 @@
       <c r="M98">
         <v>0</v>
       </c>
-    </row>
-    <row r="99" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N98">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>97</v>
       </c>
@@ -4561,8 +4858,11 @@
       <c r="M99">
         <v>0</v>
       </c>
-    </row>
-    <row r="100" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N99">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>98</v>
       </c>
@@ -4602,8 +4902,11 @@
       <c r="M100">
         <v>0</v>
       </c>
-    </row>
-    <row r="101" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N100">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>99</v>
       </c>
@@ -4643,8 +4946,11 @@
       <c r="M101">
         <v>0</v>
       </c>
-    </row>
-    <row r="102" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N101">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>100</v>
       </c>
@@ -4684,8 +4990,11 @@
       <c r="M102">
         <v>0</v>
       </c>
-    </row>
-    <row r="103" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N102">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A103">
         <v>101</v>
       </c>
@@ -4725,8 +5034,11 @@
       <c r="M103">
         <v>0</v>
       </c>
-    </row>
-    <row r="104" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N103">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A104">
         <v>102</v>
       </c>
@@ -4766,8 +5078,11 @@
       <c r="M104">
         <v>0</v>
       </c>
-    </row>
-    <row r="105" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N104">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A105">
         <v>103</v>
       </c>
@@ -4807,8 +5122,11 @@
       <c r="M105">
         <v>0</v>
       </c>
-    </row>
-    <row r="106" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N105">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>104</v>
       </c>
@@ -4848,8 +5166,11 @@
       <c r="M106">
         <v>0</v>
       </c>
-    </row>
-    <row r="107" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N106">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A107">
         <v>105</v>
       </c>
@@ -4889,8 +5210,11 @@
       <c r="M107">
         <v>0</v>
       </c>
-    </row>
-    <row r="108" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N107">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A108">
         <v>106</v>
       </c>
@@ -4930,8 +5254,11 @@
       <c r="M108">
         <v>0</v>
       </c>
-    </row>
-    <row r="109" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N108">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A109">
         <v>107</v>
       </c>
@@ -4971,8 +5298,11 @@
       <c r="M109">
         <v>0</v>
       </c>
-    </row>
-    <row r="110" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N109">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A110">
         <v>108</v>
       </c>
@@ -5012,8 +5342,11 @@
       <c r="M110">
         <v>0</v>
       </c>
-    </row>
-    <row r="111" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A111">
         <v>109</v>
       </c>
@@ -5053,8 +5386,11 @@
       <c r="M111">
         <v>0</v>
       </c>
-    </row>
-    <row r="112" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N111">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A112">
         <v>110</v>
       </c>
@@ -5094,8 +5430,11 @@
       <c r="M112">
         <v>0</v>
       </c>
-    </row>
-    <row r="113" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N112">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A113">
         <v>111</v>
       </c>
@@ -5135,8 +5474,11 @@
       <c r="M113">
         <v>0</v>
       </c>
-    </row>
-    <row r="114" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N113">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A114">
         <v>112</v>
       </c>
@@ -5176,8 +5518,11 @@
       <c r="M114">
         <v>0</v>
       </c>
-    </row>
-    <row r="115" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N114">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A115">
         <v>113</v>
       </c>
@@ -5217,8 +5562,11 @@
       <c r="M115">
         <v>0</v>
       </c>
-    </row>
-    <row r="116" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N115">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A116">
         <v>114</v>
       </c>
@@ -5258,8 +5606,11 @@
       <c r="M116">
         <v>0</v>
       </c>
-    </row>
-    <row r="117" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N116">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A117">
         <v>115</v>
       </c>
@@ -5299,8 +5650,11 @@
       <c r="M117">
         <v>0</v>
       </c>
-    </row>
-    <row r="118" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N117">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A118">
         <v>116</v>
       </c>
@@ -5340,8 +5694,11 @@
       <c r="M118">
         <v>0</v>
       </c>
-    </row>
-    <row r="119" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N118">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A119">
         <v>117</v>
       </c>
@@ -5381,8 +5738,11 @@
       <c r="M119">
         <v>0</v>
       </c>
-    </row>
-    <row r="120" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N119">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A120">
         <v>118</v>
       </c>
@@ -5422,8 +5782,11 @@
       <c r="M120">
         <v>0</v>
       </c>
-    </row>
-    <row r="121" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N120">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A121">
         <v>119</v>
       </c>
@@ -5463,8 +5826,11 @@
       <c r="M121">
         <v>0</v>
       </c>
-    </row>
-    <row r="122" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N121">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A122">
         <v>120</v>
       </c>
@@ -5504,8 +5870,11 @@
       <c r="M122">
         <v>0</v>
       </c>
-    </row>
-    <row r="123" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N122">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A123">
         <v>121</v>
       </c>
@@ -5545,8 +5914,11 @@
       <c r="M123">
         <v>0</v>
       </c>
-    </row>
-    <row r="124" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N123">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A124">
         <v>122</v>
       </c>
@@ -5586,8 +5958,11 @@
       <c r="M124">
         <v>0</v>
       </c>
-    </row>
-    <row r="125" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N124">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A125">
         <v>123</v>
       </c>
@@ -5627,8 +6002,11 @@
       <c r="M125">
         <v>0</v>
       </c>
-    </row>
-    <row r="126" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N125">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A126">
         <v>124</v>
       </c>
@@ -5668,8 +6046,11 @@
       <c r="M126">
         <v>0</v>
       </c>
-    </row>
-    <row r="127" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N126">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A127">
         <v>125</v>
       </c>
@@ -5709,8 +6090,11 @@
       <c r="M127">
         <v>0</v>
       </c>
-    </row>
-    <row r="128" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N127">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A128">
         <v>126</v>
       </c>
@@ -5750,8 +6134,11 @@
       <c r="M128">
         <v>0</v>
       </c>
-    </row>
-    <row r="129" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N128">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A129">
         <v>127</v>
       </c>
@@ -5791,8 +6178,11 @@
       <c r="M129">
         <v>0</v>
       </c>
-    </row>
-    <row r="130" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N129">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A130">
         <v>128</v>
       </c>
@@ -5832,8 +6222,11 @@
       <c r="M130">
         <v>0</v>
       </c>
-    </row>
-    <row r="131" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N130">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A131">
         <v>129</v>
       </c>
@@ -5873,8 +6266,11 @@
       <c r="M131">
         <v>0</v>
       </c>
-    </row>
-    <row r="132" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N131">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A132">
         <v>130</v>
       </c>
@@ -5914,8 +6310,11 @@
       <c r="M132">
         <v>0</v>
       </c>
-    </row>
-    <row r="133" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N132">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A133">
         <v>131</v>
       </c>
@@ -5955,8 +6354,11 @@
       <c r="M133">
         <v>0</v>
       </c>
-    </row>
-    <row r="134" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N133">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A134">
         <v>132</v>
       </c>
@@ -5996,8 +6398,11 @@
       <c r="M134">
         <v>0</v>
       </c>
-    </row>
-    <row r="135" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N134">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A135">
         <v>133</v>
       </c>
@@ -6037,8 +6442,11 @@
       <c r="M135">
         <v>0</v>
       </c>
-    </row>
-    <row r="136" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N135">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A136">
         <v>134</v>
       </c>
@@ -6078,8 +6486,11 @@
       <c r="M136">
         <v>0</v>
       </c>
-    </row>
-    <row r="137" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N136">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A137">
         <v>135</v>
       </c>
@@ -6119,8 +6530,11 @@
       <c r="M137">
         <v>0</v>
       </c>
-    </row>
-    <row r="138" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N137">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A138">
         <v>136</v>
       </c>
@@ -6160,8 +6574,11 @@
       <c r="M138">
         <v>0</v>
       </c>
-    </row>
-    <row r="139" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N138">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A139">
         <v>137</v>
       </c>
@@ -6201,8 +6618,11 @@
       <c r="M139">
         <v>0</v>
       </c>
-    </row>
-    <row r="140" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N139">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A140">
         <v>138</v>
       </c>
@@ -6242,8 +6662,11 @@
       <c r="M140">
         <v>0</v>
       </c>
-    </row>
-    <row r="141" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N140">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="141" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A141">
         <v>139</v>
       </c>
@@ -6283,8 +6706,11 @@
       <c r="M141">
         <v>0</v>
       </c>
-    </row>
-    <row r="142" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N141">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="142" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A142">
         <v>140</v>
       </c>
@@ -6324,8 +6750,11 @@
       <c r="M142">
         <v>0</v>
       </c>
-    </row>
-    <row r="143" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N142">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="143" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A143">
         <v>141</v>
       </c>
@@ -6365,8 +6794,11 @@
       <c r="M143">
         <v>0</v>
       </c>
-    </row>
-    <row r="144" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N143">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="144" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A144">
         <v>142</v>
       </c>
@@ -6406,8 +6838,11 @@
       <c r="M144">
         <v>0</v>
       </c>
-    </row>
-    <row r="145" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N144">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="145" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A145">
         <v>143</v>
       </c>
@@ -6447,8 +6882,11 @@
       <c r="M145">
         <v>0</v>
       </c>
-    </row>
-    <row r="146" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N145">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="146" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A146">
         <v>144</v>
       </c>
@@ -6488,8 +6926,11 @@
       <c r="M146">
         <v>0</v>
       </c>
-    </row>
-    <row r="147" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N146">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="147" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A147">
         <v>145</v>
       </c>
@@ -6529,8 +6970,11 @@
       <c r="M147">
         <v>0</v>
       </c>
-    </row>
-    <row r="148" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N147">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="148" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A148">
         <v>146</v>
       </c>
@@ -6570,8 +7014,11 @@
       <c r="M148">
         <v>0</v>
       </c>
-    </row>
-    <row r="149" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N148">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="149" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A149">
         <v>147</v>
       </c>
@@ -6611,8 +7058,11 @@
       <c r="M149">
         <v>0</v>
       </c>
-    </row>
-    <row r="150" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N149">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="150" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A150">
         <v>148</v>
       </c>
@@ -6652,8 +7102,11 @@
       <c r="M150">
         <v>0</v>
       </c>
-    </row>
-    <row r="151" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N150">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="151" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A151">
         <v>149</v>
       </c>
@@ -6693,8 +7146,11 @@
       <c r="M151">
         <v>0</v>
       </c>
-    </row>
-    <row r="152" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N151">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="152" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A152">
         <v>150</v>
       </c>
@@ -6734,8 +7190,11 @@
       <c r="M152">
         <v>0</v>
       </c>
-    </row>
-    <row r="153" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N152">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="153" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A153">
         <v>151</v>
       </c>
@@ -6775,8 +7234,11 @@
       <c r="M153">
         <v>0</v>
       </c>
-    </row>
-    <row r="154" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N153">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="154" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A154">
         <v>152</v>
       </c>
@@ -6816,8 +7278,11 @@
       <c r="M154">
         <v>0</v>
       </c>
-    </row>
-    <row r="155" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N154">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="155" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A155">
         <v>153</v>
       </c>
@@ -6857,8 +7322,11 @@
       <c r="M155">
         <v>0</v>
       </c>
-    </row>
-    <row r="156" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N155">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="156" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A156">
         <v>154</v>
       </c>
@@ -6898,8 +7366,11 @@
       <c r="M156">
         <v>0</v>
       </c>
-    </row>
-    <row r="157" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N156">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="157" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A157">
         <v>155</v>
       </c>
@@ -6939,8 +7410,11 @@
       <c r="M157">
         <v>0</v>
       </c>
-    </row>
-    <row r="158" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N157">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="158" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A158">
         <v>156</v>
       </c>
@@ -6980,8 +7454,11 @@
       <c r="M158">
         <v>0</v>
       </c>
-    </row>
-    <row r="159" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N158">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="159" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A159">
         <v>157</v>
       </c>
@@ -7021,8 +7498,11 @@
       <c r="M159">
         <v>0</v>
       </c>
-    </row>
-    <row r="160" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N159">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="160" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A160">
         <v>158</v>
       </c>
@@ -7062,8 +7542,11 @@
       <c r="M160">
         <v>0</v>
       </c>
-    </row>
-    <row r="161" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N160">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="161" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A161">
         <v>159</v>
       </c>
@@ -7103,8 +7586,11 @@
       <c r="M161">
         <v>0</v>
       </c>
-    </row>
-    <row r="162" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N161">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="162" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A162">
         <v>160</v>
       </c>
@@ -7144,8 +7630,11 @@
       <c r="M162">
         <v>0</v>
       </c>
-    </row>
-    <row r="163" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N162">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="163" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A163">
         <v>161</v>
       </c>
@@ -7185,8 +7674,11 @@
       <c r="M163">
         <v>0</v>
       </c>
-    </row>
-    <row r="164" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N163">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="164" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A164">
         <v>162</v>
       </c>
@@ -7226,8 +7718,11 @@
       <c r="M164">
         <v>0</v>
       </c>
-    </row>
-    <row r="165" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N164">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="165" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A165">
         <v>163</v>
       </c>
@@ -7267,8 +7762,11 @@
       <c r="M165">
         <v>0</v>
       </c>
-    </row>
-    <row r="166" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N165">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="166" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A166">
         <v>164</v>
       </c>
@@ -7308,8 +7806,11 @@
       <c r="M166">
         <v>0</v>
       </c>
-    </row>
-    <row r="167" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N166">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="167" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A167">
         <v>165</v>
       </c>
@@ -7349,8 +7850,11 @@
       <c r="M167">
         <v>0</v>
       </c>
-    </row>
-    <row r="168" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N167">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="168" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A168">
         <v>166</v>
       </c>
@@ -7390,8 +7894,11 @@
       <c r="M168">
         <v>0</v>
       </c>
-    </row>
-    <row r="169" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N168">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="169" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A169">
         <v>167</v>
       </c>
@@ -7431,8 +7938,11 @@
       <c r="M169">
         <v>0</v>
       </c>
-    </row>
-    <row r="170" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N169">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="170" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A170">
         <v>168</v>
       </c>
@@ -7472,8 +7982,11 @@
       <c r="M170">
         <v>0</v>
       </c>
-    </row>
-    <row r="171" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N170">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="171" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A171">
         <v>169</v>
       </c>
@@ -7513,8 +8026,11 @@
       <c r="M171">
         <v>0</v>
       </c>
-    </row>
-    <row r="172" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N171">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="172" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A172">
         <v>170</v>
       </c>
@@ -7554,8 +8070,11 @@
       <c r="M172">
         <v>0</v>
       </c>
-    </row>
-    <row r="173" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N172">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="173" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A173">
         <v>171</v>
       </c>
@@ -7595,8 +8114,11 @@
       <c r="M173">
         <v>0</v>
       </c>
-    </row>
-    <row r="174" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N173">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="174" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A174">
         <v>172</v>
       </c>
@@ -7636,8 +8158,11 @@
       <c r="M174">
         <v>0</v>
       </c>
-    </row>
-    <row r="175" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N174">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="175" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A175">
         <v>173</v>
       </c>
@@ -7677,8 +8202,11 @@
       <c r="M175">
         <v>0</v>
       </c>
-    </row>
-    <row r="176" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N175">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="176" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A176">
         <v>174</v>
       </c>
@@ -7718,8 +8246,11 @@
       <c r="M176">
         <v>0</v>
       </c>
-    </row>
-    <row r="177" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N176">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="177" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A177">
         <v>175</v>
       </c>
@@ -7759,8 +8290,11 @@
       <c r="M177">
         <v>0</v>
       </c>
-    </row>
-    <row r="178" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N177">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="178" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A178">
         <v>176</v>
       </c>
@@ -7800,8 +8334,11 @@
       <c r="M178">
         <v>0</v>
       </c>
-    </row>
-    <row r="179" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N178">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="179" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A179">
         <v>177</v>
       </c>
@@ -7841,8 +8378,11 @@
       <c r="M179">
         <v>0</v>
       </c>
-    </row>
-    <row r="180" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N179">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="180" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A180">
         <v>178</v>
       </c>
@@ -7882,8 +8422,11 @@
       <c r="M180">
         <v>0</v>
       </c>
-    </row>
-    <row r="181" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N180">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="181" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A181">
         <v>179</v>
       </c>
@@ -7923,8 +8466,11 @@
       <c r="M181">
         <v>0</v>
       </c>
-    </row>
-    <row r="182" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N181">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="182" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A182">
         <v>180</v>
       </c>
@@ -7964,8 +8510,11 @@
       <c r="M182">
         <v>0</v>
       </c>
-    </row>
-    <row r="183" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N182">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="183" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A183">
         <v>181</v>
       </c>
@@ -8005,8 +8554,11 @@
       <c r="M183">
         <v>0</v>
       </c>
-    </row>
-    <row r="184" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N183">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="184" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A184">
         <v>182</v>
       </c>
@@ -8046,8 +8598,11 @@
       <c r="M184">
         <v>0</v>
       </c>
-    </row>
-    <row r="185" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N184">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="185" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A185">
         <v>183</v>
       </c>
@@ -8087,8 +8642,11 @@
       <c r="M185">
         <v>0</v>
       </c>
-    </row>
-    <row r="186" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N185">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="186" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A186">
         <v>184</v>
       </c>
@@ -8128,8 +8686,11 @@
       <c r="M186">
         <v>0</v>
       </c>
-    </row>
-    <row r="187" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N186">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="187" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A187">
         <v>185</v>
       </c>
@@ -8169,8 +8730,11 @@
       <c r="M187">
         <v>0</v>
       </c>
-    </row>
-    <row r="188" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N187">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="188" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A188">
         <v>186</v>
       </c>
@@ -8210,8 +8774,11 @@
       <c r="M188">
         <v>0</v>
       </c>
-    </row>
-    <row r="189" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N188">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="189" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A189">
         <v>187</v>
       </c>
@@ -8251,8 +8818,11 @@
       <c r="M189">
         <v>0</v>
       </c>
-    </row>
-    <row r="190" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N189">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="190" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A190">
         <v>188</v>
       </c>
@@ -8292,8 +8862,11 @@
       <c r="M190">
         <v>0</v>
       </c>
-    </row>
-    <row r="191" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N190">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="191" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A191">
         <v>189</v>
       </c>
@@ -8333,8 +8906,11 @@
       <c r="M191">
         <v>0</v>
       </c>
-    </row>
-    <row r="192" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N191">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="192" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A192">
         <v>190</v>
       </c>
@@ -8374,8 +8950,11 @@
       <c r="M192">
         <v>0</v>
       </c>
-    </row>
-    <row r="193" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N192">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="193" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A193">
         <v>191</v>
       </c>
@@ -8415,8 +8994,11 @@
       <c r="M193">
         <v>0</v>
       </c>
-    </row>
-    <row r="194" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N193">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="194" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A194">
         <v>192</v>
       </c>
@@ -8456,8 +9038,11 @@
       <c r="M194">
         <v>0</v>
       </c>
-    </row>
-    <row r="195" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N194">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="195" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A195">
         <v>193</v>
       </c>
@@ -8497,8 +9082,11 @@
       <c r="M195">
         <v>0</v>
       </c>
-    </row>
-    <row r="196" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N195">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="196" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A196">
         <v>194</v>
       </c>
@@ -8538,8 +9126,11 @@
       <c r="M196">
         <v>0</v>
       </c>
-    </row>
-    <row r="197" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N196">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="197" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A197">
         <v>195</v>
       </c>
@@ -8579,8 +9170,11 @@
       <c r="M197">
         <v>0</v>
       </c>
-    </row>
-    <row r="198" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N197">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="198" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A198">
         <v>196</v>
       </c>
@@ -8620,8 +9214,11 @@
       <c r="M198">
         <v>0</v>
       </c>
-    </row>
-    <row r="199" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N198">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="199" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A199">
         <v>197</v>
       </c>
@@ -8661,8 +9258,11 @@
       <c r="M199">
         <v>0</v>
       </c>
-    </row>
-    <row r="200" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N199">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="200" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A200">
         <v>198</v>
       </c>
@@ -8702,8 +9302,11 @@
       <c r="M200">
         <v>0</v>
       </c>
-    </row>
-    <row r="201" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N200">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="201" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A201">
         <v>199</v>
       </c>
@@ -8743,8 +9346,11 @@
       <c r="M201">
         <v>0</v>
       </c>
-    </row>
-    <row r="202" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N201">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="202" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A202">
         <v>200</v>
       </c>
@@ -8784,8 +9390,11 @@
       <c r="M202">
         <v>0</v>
       </c>
-    </row>
-    <row r="203" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N202">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="203" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A203">
         <v>201</v>
       </c>
@@ -8825,8 +9434,11 @@
       <c r="M203">
         <v>0</v>
       </c>
-    </row>
-    <row r="204" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N203">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="204" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A204">
         <v>202</v>
       </c>
@@ -8866,8 +9478,11 @@
       <c r="M204">
         <v>0</v>
       </c>
-    </row>
-    <row r="205" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N204">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="205" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A205">
         <v>203</v>
       </c>
@@ -8907,8 +9522,11 @@
       <c r="M205">
         <v>0</v>
       </c>
-    </row>
-    <row r="206" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N205">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="206" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A206">
         <v>204</v>
       </c>
@@ -8948,8 +9566,11 @@
       <c r="M206">
         <v>0</v>
       </c>
-    </row>
-    <row r="207" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N206">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="207" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A207">
         <v>205</v>
       </c>
@@ -8989,8 +9610,11 @@
       <c r="M207">
         <v>0</v>
       </c>
-    </row>
-    <row r="208" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N207">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="208" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A208">
         <v>206</v>
       </c>
@@ -9030,8 +9654,11 @@
       <c r="M208">
         <v>0</v>
       </c>
-    </row>
-    <row r="209" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N208">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="209" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A209">
         <v>207</v>
       </c>
@@ -9071,8 +9698,11 @@
       <c r="M209">
         <v>0</v>
       </c>
-    </row>
-    <row r="210" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N209">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="210" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A210">
         <v>208</v>
       </c>
@@ -9112,8 +9742,11 @@
       <c r="M210">
         <v>0</v>
       </c>
-    </row>
-    <row r="211" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N210">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="211" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A211">
         <v>209</v>
       </c>
@@ -9153,8 +9786,11 @@
       <c r="M211">
         <v>0</v>
       </c>
-    </row>
-    <row r="212" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N211">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="212" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A212">
         <v>210</v>
       </c>
@@ -9194,8 +9830,11 @@
       <c r="M212">
         <v>0</v>
       </c>
-    </row>
-    <row r="213" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N212">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="213" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A213">
         <v>211</v>
       </c>
@@ -9235,8 +9874,11 @@
       <c r="M213">
         <v>0</v>
       </c>
-    </row>
-    <row r="214" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N213">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="214" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A214">
         <v>212</v>
       </c>
@@ -9276,8 +9918,11 @@
       <c r="M214">
         <v>0</v>
       </c>
-    </row>
-    <row r="215" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N214">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="215" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A215">
         <v>213</v>
       </c>
@@ -9317,8 +9962,11 @@
       <c r="M215">
         <v>0</v>
       </c>
-    </row>
-    <row r="216" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N215">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="216" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A216">
         <v>214</v>
       </c>
@@ -9358,8 +10006,11 @@
       <c r="M216">
         <v>0</v>
       </c>
-    </row>
-    <row r="217" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N216">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="217" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A217">
         <v>215</v>
       </c>
@@ -9399,8 +10050,11 @@
       <c r="M217">
         <v>0</v>
       </c>
-    </row>
-    <row r="218" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N217">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="218" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A218">
         <v>216</v>
       </c>
@@ -9440,8 +10094,11 @@
       <c r="M218">
         <v>0</v>
       </c>
-    </row>
-    <row r="219" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N218">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="219" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A219">
         <v>217</v>
       </c>
@@ -9481,8 +10138,11 @@
       <c r="M219">
         <v>0</v>
       </c>
-    </row>
-    <row r="220" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N219">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="220" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A220">
         <v>218</v>
       </c>
@@ -9522,8 +10182,11 @@
       <c r="M220">
         <v>0</v>
       </c>
-    </row>
-    <row r="221" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N220">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="221" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A221">
         <v>219</v>
       </c>
@@ -9563,8 +10226,11 @@
       <c r="M221">
         <v>0</v>
       </c>
-    </row>
-    <row r="222" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N221">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="222" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A222">
         <v>220</v>
       </c>
@@ -9604,8 +10270,11 @@
       <c r="M222">
         <v>0</v>
       </c>
-    </row>
-    <row r="223" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N222">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="223" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A223">
         <v>221</v>
       </c>
@@ -9645,8 +10314,11 @@
       <c r="M223">
         <v>0</v>
       </c>
-    </row>
-    <row r="224" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N223">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="224" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A224">
         <v>222</v>
       </c>
@@ -9686,8 +10358,11 @@
       <c r="M224">
         <v>0</v>
       </c>
-    </row>
-    <row r="225" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N224">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="225" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A225">
         <v>223</v>
       </c>
@@ -9727,8 +10402,11 @@
       <c r="M225">
         <v>0</v>
       </c>
-    </row>
-    <row r="226" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N225">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="226" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A226">
         <v>224</v>
       </c>
@@ -9768,8 +10446,11 @@
       <c r="M226">
         <v>0</v>
       </c>
-    </row>
-    <row r="227" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N226">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="227" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A227">
         <v>225</v>
       </c>
@@ -9809,8 +10490,11 @@
       <c r="M227">
         <v>0</v>
       </c>
-    </row>
-    <row r="228" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N227">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="228" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A228">
         <v>226</v>
       </c>
@@ -9850,8 +10534,11 @@
       <c r="M228">
         <v>0</v>
       </c>
-    </row>
-    <row r="229" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N228">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="229" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A229">
         <v>227</v>
       </c>
@@ -9891,8 +10578,11 @@
       <c r="M229">
         <v>0</v>
       </c>
-    </row>
-    <row r="230" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N229">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="230" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A230">
         <v>228</v>
       </c>
@@ -9932,8 +10622,11 @@
       <c r="M230">
         <v>0</v>
       </c>
-    </row>
-    <row r="231" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N230">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="231" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A231">
         <v>229</v>
       </c>
@@ -9973,8 +10666,11 @@
       <c r="M231">
         <v>0</v>
       </c>
-    </row>
-    <row r="232" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N231">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="232" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A232">
         <v>230</v>
       </c>
@@ -10014,8 +10710,11 @@
       <c r="M232">
         <v>0</v>
       </c>
-    </row>
-    <row r="233" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N232">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="233" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A233">
         <v>231</v>
       </c>
@@ -10055,8 +10754,11 @@
       <c r="M233">
         <v>0</v>
       </c>
-    </row>
-    <row r="234" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N233">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="234" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A234">
         <v>232</v>
       </c>
@@ -10096,8 +10798,11 @@
       <c r="M234">
         <v>0</v>
       </c>
-    </row>
-    <row r="235" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N234">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="235" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A235">
         <v>233</v>
       </c>
@@ -10137,8 +10842,11 @@
       <c r="M235">
         <v>0</v>
       </c>
-    </row>
-    <row r="236" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N235">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="236" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A236">
         <v>234</v>
       </c>
@@ -10178,8 +10886,11 @@
       <c r="M236">
         <v>0</v>
       </c>
-    </row>
-    <row r="237" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N236">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="237" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A237">
         <v>235</v>
       </c>
@@ -10219,8 +10930,11 @@
       <c r="M237">
         <v>0</v>
       </c>
-    </row>
-    <row r="238" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N237">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="238" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A238">
         <v>236</v>
       </c>
@@ -10260,8 +10974,11 @@
       <c r="M238">
         <v>0</v>
       </c>
-    </row>
-    <row r="239" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N238">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="239" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A239">
         <v>237</v>
       </c>
@@ -10301,8 +11018,11 @@
       <c r="M239">
         <v>0</v>
       </c>
-    </row>
-    <row r="240" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N239">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="240" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A240">
         <v>238</v>
       </c>
@@ -10342,8 +11062,11 @@
       <c r="M240">
         <v>0</v>
       </c>
-    </row>
-    <row r="241" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N240">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="241" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A241">
         <v>239</v>
       </c>
@@ -10383,8 +11106,11 @@
       <c r="M241">
         <v>0</v>
       </c>
-    </row>
-    <row r="242" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N241">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="242" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A242">
         <v>240</v>
       </c>
@@ -10424,8 +11150,11 @@
       <c r="M242">
         <v>0</v>
       </c>
-    </row>
-    <row r="243" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N242">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="243" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A243">
         <v>241</v>
       </c>
@@ -10465,8 +11194,11 @@
       <c r="M243">
         <v>0</v>
       </c>
-    </row>
-    <row r="244" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N243">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="244" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A244">
         <v>242</v>
       </c>
@@ -10506,8 +11238,11 @@
       <c r="M244">
         <v>0</v>
       </c>
-    </row>
-    <row r="245" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N244">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="245" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A245">
         <v>243</v>
       </c>
@@ -10547,8 +11282,11 @@
       <c r="M245">
         <v>0</v>
       </c>
-    </row>
-    <row r="246" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N245">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="246" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A246">
         <v>244</v>
       </c>
@@ -10588,8 +11326,11 @@
       <c r="M246">
         <v>0</v>
       </c>
-    </row>
-    <row r="247" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N246">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="247" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A247">
         <v>245</v>
       </c>
@@ -10629,8 +11370,11 @@
       <c r="M247">
         <v>0</v>
       </c>
-    </row>
-    <row r="248" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N247">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="248" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A248">
         <v>246</v>
       </c>
@@ -10670,8 +11414,11 @@
       <c r="M248">
         <v>0</v>
       </c>
-    </row>
-    <row r="249" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N248">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="249" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A249">
         <v>247</v>
       </c>
@@ -10711,8 +11458,11 @@
       <c r="M249">
         <v>0</v>
       </c>
-    </row>
-    <row r="250" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N249">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="250" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A250">
         <v>248</v>
       </c>
@@ -10752,8 +11502,11 @@
       <c r="M250">
         <v>0</v>
       </c>
-    </row>
-    <row r="251" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N250">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="251" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A251">
         <v>249</v>
       </c>
@@ -10793,8 +11546,11 @@
       <c r="M251">
         <v>0</v>
       </c>
-    </row>
-    <row r="252" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N251">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="252" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A252">
         <v>250</v>
       </c>
@@ -10834,8 +11590,11 @@
       <c r="M252">
         <v>0</v>
       </c>
-    </row>
-    <row r="253" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N252">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="253" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A253">
         <v>251</v>
       </c>
@@ -10875,8 +11634,11 @@
       <c r="M253">
         <v>0</v>
       </c>
-    </row>
-    <row r="254" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N253">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="254" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A254">
         <v>252</v>
       </c>
@@ -10916,8 +11678,11 @@
       <c r="M254">
         <v>0</v>
       </c>
-    </row>
-    <row r="255" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N254">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="255" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A255">
         <v>253</v>
       </c>
@@ -10957,8 +11722,11 @@
       <c r="M255">
         <v>0</v>
       </c>
-    </row>
-    <row r="256" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N255">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="256" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A256">
         <v>254</v>
       </c>
@@ -10998,8 +11766,11 @@
       <c r="M256">
         <v>17</v>
       </c>
-    </row>
-    <row r="257" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N256">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="257" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A257">
         <v>255</v>
       </c>
@@ -11037,6 +11808,9 @@
         <v>0</v>
       </c>
       <c r="M257">
+        <v>0</v>
+      </c>
+      <c r="N257">
         <v>0</v>
       </c>
     </row>
@@ -11047,7 +11821,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33C90694-17B9-4987-A12B-4F203B0E59C7}">
-  <dimension ref="A1:M5"/>
+  <dimension ref="A1:N5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="M2" sqref="M2:M5"/>
@@ -11055,7 +11829,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>15</v>
       </c>
@@ -11092,8 +11866,11 @@
       <c r="M1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -11122,7 +11899,7 @@
         <v>36</v>
       </c>
       <c r="J2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="K2">
         <v>17</v>
@@ -11133,8 +11910,11 @@
       <c r="M2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -11174,8 +11954,11 @@
       <c r="M3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -11215,8 +11998,11 @@
       <c r="M4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -11254,6 +12040,9 @@
         <v>37</v>
       </c>
       <c r="M5" t="s">
+        <v>37</v>
+      </c>
+      <c r="N5" t="s">
         <v>37</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Link GUI script with startSimulation Script
</commit_message>
<xml_diff>
--- a/memory.xlsx
+++ b/memory.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB04E790-0285-4AB3-A7DD-8389BA255F16}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7790E41A-372E-4BC0-8691-915021D873B5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="312" yWindow="312" windowWidth="22728" windowHeight="12048" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>

</xml_diff>